<commit_message>
initial 24 hour data
</commit_message>
<xml_diff>
--- a/Experiment_Collection.xlsx
+++ b/Experiment_Collection.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobnelson/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cjannusch/Desktop/Schoolwork/STAT424/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CDEB8434-0F80-BE41-95D1-12C22E27B704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C938B6CA-E6B0-A145-AB74-C24189C6D206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16080" xr2:uid="{581E7E5D-B6B6-BD48-AC8D-EFEAD386A768}"/>
+    <workbookView xWindow="3820" yWindow="1300" windowWidth="28040" windowHeight="16080" xr2:uid="{581E7E5D-B6B6-BD48-AC8D-EFEAD386A768}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="16">
   <si>
     <t>Hardwood_Type</t>
   </si>
@@ -48,12 +48,6 @@
     <t>Mass_After</t>
   </si>
   <si>
-    <t>Oak</t>
-  </si>
-  <si>
-    <t>Maple</t>
-  </si>
-  <si>
     <t>Cherry</t>
   </si>
   <si>
@@ -61,6 +55,33 @@
   </si>
   <si>
     <t>Ash</t>
+  </si>
+  <si>
+    <t>White Birch</t>
+  </si>
+  <si>
+    <t>Pine</t>
+  </si>
+  <si>
+    <t>Cherry (1)</t>
+  </si>
+  <si>
+    <t>Walnut (2)</t>
+  </si>
+  <si>
+    <t>Ash (3)</t>
+  </si>
+  <si>
+    <t>White Birch (4)</t>
+  </si>
+  <si>
+    <t>Pine (5)</t>
+  </si>
+  <si>
+    <t>% Increase After a Day</t>
+  </si>
+  <si>
+    <t>Average per Type</t>
   </si>
 </sst>
 </file>
@@ -102,7 +123,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -116,13 +144,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7EF4DA9F-985D-CF48-8BE3-0E427618994A}" name="Table2" displayName="Table2" ref="A1:D41" totalsRowShown="0">
-  <autoFilter ref="A1:D41" xr:uid="{7EF4DA9F-985D-CF48-8BE3-0E427618994A}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7EF4DA9F-985D-CF48-8BE3-0E427618994A}" name="Table2" displayName="Table2" ref="A1:F41" totalsRowShown="0">
+  <autoFilter ref="A1:F41" xr:uid="{7EF4DA9F-985D-CF48-8BE3-0E427618994A}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{AEAD3080-15EC-F848-BAA2-45DD8F322B56}" name="Hardwood_Type"/>
     <tableColumn id="2" xr3:uid="{95F96CDC-5EF4-1542-B5D4-A1E7C5DBE86B}" name="Replicate_No"/>
     <tableColumn id="3" xr3:uid="{75F672B3-023A-CB43-B4E6-E93086399089}" name="Mass_Before"/>
     <tableColumn id="4" xr3:uid="{40182514-4A49-8D4A-9008-990BF1C9864C}" name="Mass_After"/>
+    <tableColumn id="5" xr3:uid="{2BB2B80A-4760-4940-B8B7-1296CC334437}" name="% Increase After a Day" dataDxfId="1">
+      <calculatedColumnFormula>(Table2[[#This Row],[Mass_After]]-Table2[[#This Row],[Mass_Before]])/Table2[[#This Row],[Mass_Before]]*100</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{08C84FF7-466C-F341-8105-B6C3BE919DE8}" name="Average per Type" dataDxfId="0">
+      <calculatedColumnFormula>AVERAGE(E2:E6)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -425,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDEFEB39-FAA5-414D-9E12-CD9931844F25}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -437,9 +471,11 @@
     <col min="2" max="2" width="15.1640625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -452,325 +488,481 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>48</v>
+      </c>
+      <c r="D2">
+        <v>58</v>
+      </c>
+      <c r="E2">
+        <f>(Table2[[#This Row],[Mass_After]]-Table2[[#This Row],[Mass_Before]])/Table2[[#This Row],[Mass_Before]]*100</f>
+        <v>20.833333333333336</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ref="F2:F41" si="0">AVERAGE(E2:E6)</f>
+        <v>23.411111111111111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>27</v>
+      </c>
+      <c r="D3">
+        <v>33</v>
+      </c>
+      <c r="E3">
+        <f>(Table2[[#This Row],[Mass_After]]-Table2[[#This Row],[Mass_Before]])/Table2[[#This Row],[Mass_Before]]*100</f>
+        <v>22.222222222222221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>25</v>
+      </c>
+      <c r="D4">
+        <v>31</v>
+      </c>
+      <c r="E4">
+        <f>(Table2[[#This Row],[Mass_After]]-Table2[[#This Row],[Mass_Before]])/Table2[[#This Row],[Mass_Before]]*100</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>26</v>
+      </c>
+      <c r="D5">
+        <v>33</v>
+      </c>
+      <c r="E5">
+        <f>(Table2[[#This Row],[Mass_After]]-Table2[[#This Row],[Mass_Before]])/Table2[[#This Row],[Mass_Before]]*100</f>
+        <v>26.923076923076923</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>26</v>
+      </c>
+      <c r="D6">
+        <v>32</v>
+      </c>
+      <c r="E6">
+        <f>(Table2[[#This Row],[Mass_After]]-Table2[[#This Row],[Mass_Before]])/Table2[[#This Row],[Mass_Before]]*100</f>
+        <v>23.076923076923077</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>60</v>
+      </c>
+      <c r="D7">
+        <v>72</v>
+      </c>
+      <c r="E7">
+        <f>(Table2[[#This Row],[Mass_After]]-Table2[[#This Row],[Mass_Before]])/Table2[[#This Row],[Mass_Before]]*100</f>
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>22.213705463983551</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>30</v>
+      </c>
+      <c r="D8">
+        <v>37</v>
+      </c>
+      <c r="E8">
+        <f>(Table2[[#This Row],[Mass_After]]-Table2[[#This Row],[Mass_Before]])/Table2[[#This Row],[Mass_Before]]*100</f>
+        <v>23.333333333333332</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>31</v>
+      </c>
+      <c r="D9">
+        <v>37</v>
+      </c>
+      <c r="E9">
+        <f>(Table2[[#This Row],[Mass_After]]-Table2[[#This Row],[Mass_Before]])/Table2[[#This Row],[Mass_Before]]*100</f>
+        <v>19.35483870967742</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
       <c r="B10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>29</v>
+      </c>
+      <c r="D10">
+        <v>36</v>
+      </c>
+      <c r="E10">
+        <f>(Table2[[#This Row],[Mass_After]]-Table2[[#This Row],[Mass_Before]])/Table2[[#This Row],[Mass_Before]]*100</f>
+        <v>24.137931034482758</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>5</v>
       </c>
       <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>33</v>
+      </c>
+      <c r="D11">
+        <v>41</v>
+      </c>
+      <c r="E11">
+        <f>(Table2[[#This Row],[Mass_After]]-Table2[[#This Row],[Mass_Before]])/Table2[[#This Row],[Mass_Before]]*100</f>
+        <v>24.242424242424242</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>53</v>
+      </c>
+      <c r="D12">
+        <v>64</v>
+      </c>
+      <c r="E12">
+        <f>(Table2[[#This Row],[Mass_After]]-Table2[[#This Row],[Mass_Before]])/Table2[[#This Row],[Mass_Before]]*100</f>
+        <v>20.754716981132077</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>28.968273192866558</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="C13">
+        <v>26</v>
+      </c>
+      <c r="D13">
+        <v>35</v>
+      </c>
+      <c r="E13">
+        <f>(Table2[[#This Row],[Mass_After]]-Table2[[#This Row],[Mass_Before]])/Table2[[#This Row],[Mass_Before]]*100</f>
+        <v>34.615384615384613</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>29</v>
+      </c>
+      <c r="D14">
+        <v>36</v>
+      </c>
+      <c r="E14">
+        <f>(Table2[[#This Row],[Mass_After]]-Table2[[#This Row],[Mass_Before]])/Table2[[#This Row],[Mass_Before]]*100</f>
+        <v>24.137931034482758</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>25</v>
+      </c>
+      <c r="D15">
+        <v>33</v>
+      </c>
+      <c r="E15">
+        <f>(Table2[[#This Row],[Mass_After]]-Table2[[#This Row],[Mass_Before]])/Table2[[#This Row],[Mass_Before]]*100</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16">
         <v>5</v>
       </c>
-      <c r="B12">
+      <c r="C16">
+        <v>27</v>
+      </c>
+      <c r="D16">
+        <v>36</v>
+      </c>
+      <c r="E16">
+        <f>(Table2[[#This Row],[Mass_After]]-Table2[[#This Row],[Mass_Before]])/Table2[[#This Row],[Mass_Before]]*100</f>
+        <v>33.333333333333329</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>70</v>
+      </c>
+      <c r="D17">
+        <v>92</v>
+      </c>
+      <c r="E17">
+        <f>(Table2[[#This Row],[Mass_After]]-Table2[[#This Row],[Mass_Before]])/Table2[[#This Row],[Mass_Before]]*100</f>
+        <v>31.428571428571427</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>33.692858271805633</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>38</v>
+      </c>
+      <c r="D18">
+        <v>51</v>
+      </c>
+      <c r="E18">
+        <f>(Table2[[#This Row],[Mass_After]]-Table2[[#This Row],[Mass_Before]])/Table2[[#This Row],[Mass_Before]]*100</f>
+        <v>34.210526315789473</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="C19">
+        <v>37</v>
+      </c>
+      <c r="D19">
+        <v>50</v>
+      </c>
+      <c r="E19">
+        <f>(Table2[[#This Row],[Mass_After]]-Table2[[#This Row],[Mass_Before]])/Table2[[#This Row],[Mass_Before]]*100</f>
+        <v>35.135135135135137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>38</v>
+      </c>
+      <c r="D20">
+        <v>50</v>
+      </c>
+      <c r="E20">
+        <f>(Table2[[#This Row],[Mass_After]]-Table2[[#This Row],[Mass_Before]])/Table2[[#This Row],[Mass_Before]]*100</f>
+        <v>31.578947368421051</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21">
         <v>5</v>
       </c>
-      <c r="B13">
+      <c r="C21">
+        <v>36</v>
+      </c>
+      <c r="D21">
+        <v>49</v>
+      </c>
+      <c r="E21">
+        <f>(Table2[[#This Row],[Mass_After]]-Table2[[#This Row],[Mass_Before]])/Table2[[#This Row],[Mass_Before]]*100</f>
+        <v>36.111111111111107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>56</v>
+      </c>
+      <c r="D22">
+        <v>65</v>
+      </c>
+      <c r="E22">
+        <f>(Table2[[#This Row],[Mass_After]]-Table2[[#This Row],[Mass_Before]])/Table2[[#This Row],[Mass_Before]]*100</f>
+        <v>16.071428571428573</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>19.267364181157284</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>29</v>
+      </c>
+      <c r="D23">
+        <v>34</v>
+      </c>
+      <c r="E23">
+        <f>(Table2[[#This Row],[Mass_After]]-Table2[[#This Row],[Mass_Before]])/Table2[[#This Row],[Mass_Before]]*100</f>
+        <v>17.241379310344829</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <v>28</v>
+      </c>
+      <c r="D24">
+        <v>34</v>
+      </c>
+      <c r="E24">
+        <f>(Table2[[#This Row],[Mass_After]]-Table2[[#This Row],[Mass_Before]])/Table2[[#This Row],[Mass_Before]]*100</f>
+        <v>21.428571428571427</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="C25">
+        <v>27</v>
+      </c>
+      <c r="D25">
+        <v>32</v>
+      </c>
+      <c r="E25">
+        <f>(Table2[[#This Row],[Mass_After]]-Table2[[#This Row],[Mass_Before]])/Table2[[#This Row],[Mass_Before]]*100</f>
+        <v>18.518518518518519</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26">
         <v>5</v>
       </c>
-      <c r="B14">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>7</v>
-      </c>
-      <c r="B27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>7</v>
-      </c>
-      <c r="B33">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>8</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>8</v>
-      </c>
-      <c r="B35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>8</v>
-      </c>
-      <c r="B36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>8</v>
-      </c>
-      <c r="B37">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>8</v>
-      </c>
-      <c r="B38">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>8</v>
-      </c>
-      <c r="B39">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B40">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>8</v>
-      </c>
-      <c r="B41">
-        <v>8</v>
+      <c r="C26">
+        <v>26</v>
+      </c>
+      <c r="D26">
+        <v>32</v>
+      </c>
+      <c r="E26">
+        <f>(Table2[[#This Row],[Mass_After]]-Table2[[#This Row],[Mass_Before]])/Table2[[#This Row],[Mass_Before]]*100</f>
+        <v>23.076923076923077</v>
       </c>
     </row>
   </sheetData>

</xml_diff>